<commit_message>
Add db scripts to package.json
</commit_message>
<xml_diff>
--- a/docs/data/answers/answers.xlsx
+++ b/docs/data/answers/answers.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="102">
   <si>
     <t>id</t>
   </si>
@@ -312,9 +312,6 @@
   </si>
   <si>
     <t>4bf58dd8d48988d1cd941735</t>
-  </si>
-  <si>
-    <t>european</t>
   </si>
   <si>
     <t>4bf58dd8d48988d1be941735</t>
@@ -668,7 +665,7 @@
   <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -706,7 +703,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -733,7 +730,7 @@
         <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -748,7 +745,7 @@
         <v>9</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -778,7 +775,7 @@
         <v>11</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -805,7 +802,7 @@
         <v>13</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -820,7 +817,7 @@
         <v>14</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -834,9 +831,6 @@
       <c r="C11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>96</v>
-      </c>
     </row>
     <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A12">

</xml_diff>

<commit_message>
add styling to question buttons
</commit_message>
<xml_diff>
--- a/docs/data/answers/answers.xlsx
+++ b/docs/data/answers/answers.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26709"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/syriebianco/Desktop/Programming/TellMeWhatToEat/docs/data/answers/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-320" yWindow="-21140" windowWidth="17160" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="29600" windowHeight="19060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Answers" sheetId="10" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -24,7 +19,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="109">
+  <si>
+    <t>http://res.cloudinary.com/dluh2fsyd/image/upload/v1502494739/weather_nnq91s.png</t>
+  </si>
+  <si>
+    <t>http://res.cloudinary.com/dluh2fsyd/image/upload/v1502558747/salad_fqvp16.svg</t>
+  </si>
+  <si>
+    <t>http://res.cloudinary.com/dluh2fsyd/image/upload/v1502558675/sushi_abv72i.svg</t>
+  </si>
+  <si>
+    <t>http://res.cloudinary.com/dluh2fsyd/image/upload/v1502558768/sandwhich_mbsazy.png</t>
+  </si>
   <si>
     <t>id</t>
   </si>
@@ -333,13 +340,20 @@
   </si>
   <si>
     <t>hot</t>
+  </si>
+  <si>
+    <t>img_url</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://res.cloudinary.com/dluh2fsyd/image/upload/v1502494736/Hot-Food-Icon-1_mkl4va.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -358,6 +372,10 @@
       <sz val="13"/>
       <color rgb="FFCB763C"/>
       <name val="Courier"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Verdana"/>
     </font>
   </fonts>
   <fills count="2">
@@ -390,7 +408,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -442,7 +460,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -477,7 +495,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -654,48 +672,51 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:E62"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="19.1640625" customWidth="1"/>
     <col min="4" max="4" width="29.1640625" customWidth="1"/>
     <col min="5" max="5" width="34.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
@@ -703,13 +724,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+      <c r="F2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="3" customFormat="1">
       <c r="A3" s="3">
         <f>IF(ISBLANK(B3), "", A2+1)</f>
         <v>2</v>
@@ -718,10 +742,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <f>IF(ISBLANK(B4), "", A3+1)</f>
         <v>3</v>
@@ -730,13 +757,16 @@
         <v>101</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5">
         <f>IF(ISBLANK(B5), "", A4+1)</f>
         <v>4</v>
@@ -745,13 +775,16 @@
         <v>101</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6">
         <f t="shared" ref="A6:A7" si="0">IF(ISBLANK(B6), "", A5+1)</f>
         <v>5</v>
@@ -760,13 +793,16 @@
         <v>101</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+      <c r="F6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -775,13 +811,13 @@
         <v>102</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="3" customFormat="1">
       <c r="A8" s="3">
         <f>IF(ISBLANK(B8), "", A7+1)</f>
         <v>7</v>
@@ -790,10 +826,10 @@
         <v>2</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9">
         <f t="shared" ref="A9:A25" si="1">IF(ISBLANK(B9), "", A8+1)</f>
         <v>8</v>
@@ -802,13 +838,13 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="18" customHeight="1">
       <c r="A10">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -817,13 +853,13 @@
         <v>201</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="3" customFormat="1">
       <c r="A11" s="3">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -832,13 +868,13 @@
         <v>201</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -847,13 +883,13 @@
         <v>201</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -862,13 +898,13 @@
         <v>20101</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -877,13 +913,13 @@
         <v>20101</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -892,13 +928,13 @@
         <v>2010101</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -907,13 +943,13 @@
         <v>20102</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -922,13 +958,13 @@
         <v>2010201</v>
       </c>
       <c r="C17" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E17" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -937,13 +973,13 @@
         <v>20103</v>
       </c>
       <c r="C18" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19">
         <f t="shared" si="1"/>
         <v>18</v>
@@ -952,13 +988,13 @@
         <v>20103</v>
       </c>
       <c r="C19" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20">
         <f t="shared" si="1"/>
         <v>19</v>
@@ -967,13 +1003,13 @@
         <v>20104</v>
       </c>
       <c r="C20" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -982,13 +1018,13 @@
         <v>20104</v>
       </c>
       <c r="C21" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22">
         <f t="shared" si="1"/>
         <v>21</v>
@@ -997,13 +1033,13 @@
         <v>202</v>
       </c>
       <c r="C22" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -1012,13 +1048,13 @@
         <v>202</v>
       </c>
       <c r="C23" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24">
         <f t="shared" si="1"/>
         <v>23</v>
@@ -1027,13 +1063,13 @@
         <v>20201</v>
       </c>
       <c r="C24" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -1042,13 +1078,13 @@
         <v>20201</v>
       </c>
       <c r="C25" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26">
         <f t="shared" ref="A26:A27" si="2">IF(ISBLANK(B26), "", A25+1)</f>
         <v>25</v>
@@ -1057,13 +1093,13 @@
         <v>20203</v>
       </c>
       <c r="C26" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E26" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27">
         <f t="shared" si="2"/>
         <v>26</v>
@@ -1072,10 +1108,10 @@
         <v>3</v>
       </c>
       <c r="C27" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28">
         <f t="shared" ref="A28:A62" si="3">IF(ISBLANK(B28), "", A27+1)</f>
         <v>27</v>
@@ -1084,13 +1120,13 @@
         <v>3</v>
       </c>
       <c r="C28" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29">
         <f t="shared" si="3"/>
         <v>28</v>
@@ -1099,13 +1135,13 @@
         <v>301</v>
       </c>
       <c r="C29" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30">
         <f t="shared" si="3"/>
         <v>29</v>
@@ -1114,13 +1150,13 @@
         <v>302</v>
       </c>
       <c r="C30" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31">
         <f t="shared" si="3"/>
         <v>30</v>
@@ -1129,13 +1165,13 @@
         <v>4</v>
       </c>
       <c r="C31" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D31" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32">
         <f t="shared" si="3"/>
         <v>31</v>
@@ -1144,13 +1180,13 @@
         <v>4</v>
       </c>
       <c r="C32" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D32" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33">
         <f t="shared" si="3"/>
         <v>32</v>
@@ -1159,13 +1195,13 @@
         <v>5</v>
       </c>
       <c r="C33" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D33" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34">
         <f t="shared" si="3"/>
         <v>33</v>
@@ -1174,13 +1210,13 @@
         <v>6</v>
       </c>
       <c r="C34" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D34" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35">
         <f t="shared" si="3"/>
         <v>34</v>
@@ -1189,13 +1225,13 @@
         <v>7</v>
       </c>
       <c r="C35" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36">
         <f t="shared" si="3"/>
         <v>35</v>
@@ -1204,13 +1240,13 @@
         <v>8</v>
       </c>
       <c r="C36" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D36" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37">
         <f t="shared" si="3"/>
         <v>36</v>
@@ -1219,13 +1255,13 @@
         <v>8</v>
       </c>
       <c r="C37" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38">
         <f t="shared" si="3"/>
         <v>37</v>
@@ -1234,13 +1270,13 @@
         <v>9</v>
       </c>
       <c r="C38" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D38" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39">
         <f t="shared" si="3"/>
         <v>38</v>
@@ -1249,13 +1285,13 @@
         <v>9</v>
       </c>
       <c r="C39" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D39" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40">
         <f t="shared" si="3"/>
         <v>39</v>
@@ -1264,13 +1300,13 @@
         <v>9</v>
       </c>
       <c r="C40" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41">
         <f t="shared" si="3"/>
         <v>40</v>
@@ -1279,13 +1315,13 @@
         <v>901</v>
       </c>
       <c r="C41" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D41" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
       <c r="A42">
         <f t="shared" si="3"/>
         <v>41</v>
@@ -1294,13 +1330,13 @@
         <v>901</v>
       </c>
       <c r="C42" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D42" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
       <c r="A43">
         <f t="shared" si="3"/>
         <v>42</v>
@@ -1309,13 +1345,13 @@
         <v>901</v>
       </c>
       <c r="C43" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D43" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44">
         <f t="shared" si="3"/>
         <v>43</v>
@@ -1324,13 +1360,13 @@
         <v>902</v>
       </c>
       <c r="C44" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="D44" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
       <c r="A45">
         <f t="shared" si="3"/>
         <v>44</v>
@@ -1339,13 +1375,13 @@
         <v>902</v>
       </c>
       <c r="C45" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D45" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
       <c r="A46">
         <f t="shared" si="3"/>
         <v>45</v>
@@ -1354,13 +1390,13 @@
         <v>902</v>
       </c>
       <c r="C46" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D46" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
       <c r="A47">
         <f t="shared" si="3"/>
         <v>46</v>
@@ -1369,13 +1405,13 @@
         <v>10</v>
       </c>
       <c r="C47" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D47" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
       <c r="A48">
         <f t="shared" si="3"/>
         <v>47</v>
@@ -1384,13 +1420,13 @@
         <v>10</v>
       </c>
       <c r="C48" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D48" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
       <c r="A49">
         <f t="shared" si="3"/>
         <v>48</v>
@@ -1399,13 +1435,13 @@
         <v>10</v>
       </c>
       <c r="C49" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D49" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
       <c r="A50">
         <f t="shared" si="3"/>
         <v>49</v>
@@ -1414,13 +1450,13 @@
         <v>11</v>
       </c>
       <c r="C50" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
       <c r="A51">
         <f t="shared" si="3"/>
         <v>50</v>
@@ -1429,13 +1465,13 @@
         <v>11</v>
       </c>
       <c r="C51" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
       <c r="A52">
         <f t="shared" si="3"/>
         <v>51</v>
@@ -1444,13 +1480,13 @@
         <v>12</v>
       </c>
       <c r="C52" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
       <c r="A53">
         <f t="shared" si="3"/>
         <v>52</v>
@@ -1459,13 +1495,13 @@
         <v>13</v>
       </c>
       <c r="C53" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
       <c r="A54">
         <f t="shared" si="3"/>
         <v>53</v>
@@ -1474,13 +1510,13 @@
         <v>14</v>
       </c>
       <c r="C54" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D54" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
       <c r="A55">
         <f t="shared" si="3"/>
         <v>54</v>
@@ -1489,55 +1525,61 @@
         <v>15</v>
       </c>
       <c r="C55" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="D55" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
       <c r="A56" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5">
       <c r="A57" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5">
       <c r="A58" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5">
       <c r="A59" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5">
       <c r="A60" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5">
       <c r="A61" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5">
       <c r="A62" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix positoning on landing page
</commit_message>
<xml_diff>
--- a/docs/data/answers/answers.xlsx
+++ b/docs/data/answers/answers.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26709"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/syriebianco/Desktop/Programming/TellMeWhatToEat/docs/data/answers/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="-80" windowWidth="15660" windowHeight="19060" tabRatio="500"/>
+    <workbookView xWindow="680" yWindow="460" windowWidth="27880" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Answers" sheetId="10" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="130407" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="138">
   <si>
     <t>http://res.cloudinary.com/dluh2fsyd/image/upload/v1502571352/kosher-symbol_vsjmun.png</t>
   </si>
@@ -433,19 +438,16 @@
   </si>
   <si>
     <t>4bf58dd8d48988d110941735</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4bf58dd8d48988d14e941735 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -507,7 +509,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -771,31 +773,31 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57:XFD57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="19.1640625" customWidth="1"/>
     <col min="4" max="4" width="29.1640625" customWidth="1"/>
     <col min="5" max="5" width="34.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>44</v>
       </c>
@@ -815,7 +817,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -832,7 +834,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="3" customFormat="1">
+    <row r="3" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -846,7 +848,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -863,7 +865,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -880,7 +882,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -897,7 +899,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -911,7 +913,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="3" customFormat="1">
+    <row r="8" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -922,7 +924,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="3" customFormat="1">
+    <row r="9" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -932,8 +934,11 @@
       <c r="C9" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="E9" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -947,7 +952,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="18" customHeight="1">
+    <row r="11" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -961,7 +966,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="3" customFormat="1">
+    <row r="12" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -975,7 +980,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -989,7 +994,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -1006,7 +1011,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -1023,7 +1028,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -1037,7 +1042,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -1051,7 +1056,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -1065,7 +1070,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -1082,7 +1087,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -1099,7 +1104,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -1116,7 +1121,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -1133,7 +1138,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -1150,7 +1155,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -1167,7 +1172,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -1184,7 +1189,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -1201,7 +1206,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -1215,7 +1220,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -1229,7 +1234,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -1246,7 +1251,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -1260,7 +1265,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -1274,7 +1279,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -1291,7 +1296,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -1308,7 +1313,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -1321,8 +1326,11 @@
       <c r="D34" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="35" spans="1:6">
+      <c r="E34" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -1339,7 +1347,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -1353,7 +1361,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -1370,7 +1378,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -1387,7 +1395,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -1404,7 +1412,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -1421,7 +1429,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -1438,7 +1446,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -1455,7 +1463,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -1472,7 +1480,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -1489,7 +1497,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -1506,7 +1514,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -1523,7 +1531,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -1540,7 +1548,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -1557,7 +1565,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -1574,7 +1582,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -1591,7 +1599,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -1608,7 +1616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -1625,7 +1633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -1642,7 +1650,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -1656,7 +1664,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -1670,7 +1678,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -1684,44 +1692,38 @@
         <v>135</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="str">
-        <f t="shared" ref="A29:A63" si="0">IF(ISBLANK(B57), "", A56+1)</f>
+        <f>IF(ISBLANK(B57), "",#REF!+ 1)</f>
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="A58:A62" si="0">IF(ISBLANK(B58), "", A57+1)</f>
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="63" spans="1:6">
-      <c r="A63" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -1730,10 +1732,5 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix npm run excel
</commit_message>
<xml_diff>
--- a/docs/data/answers/answers.xlsx
+++ b/docs/data/answers/answers.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="680" yWindow="460" windowWidth="27880" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27920" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Answers" sheetId="10" r:id="rId1"/>
@@ -176,9 +176,6 @@
     <t>text</t>
   </si>
   <si>
-    <t>category_ids</t>
-  </si>
-  <si>
     <t>Hot</t>
   </si>
   <si>
@@ -441,6 +438,9 @@
   </si>
   <si>
     <t xml:space="preserve"> 4bf58dd8d48988d14e941735 </t>
+  </si>
+  <si>
+    <t>category_id</t>
   </si>
 </sst>
 </file>
@@ -786,8 +786,8 @@
   </sheetPr>
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57:XFD57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -811,7 +811,7 @@
         <v>46</v>
       </c>
       <c r="E1" t="s">
-        <v>49</v>
+        <v>137</v>
       </c>
       <c r="F1" t="s">
         <v>17</v>
@@ -825,7 +825,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
@@ -842,7 +842,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>40</v>
@@ -856,7 +856,7 @@
         <v>101</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>15</v>
@@ -873,7 +873,7 @@
         <v>101</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>14</v>
@@ -890,10 +890,10 @@
         <v>101</v>
       </c>
       <c r="C6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F6" t="s">
         <v>42</v>
@@ -907,7 +907,7 @@
         <v>102</v>
       </c>
       <c r="C7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>13</v>
@@ -935,7 +935,7 @@
         <v>20</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -946,7 +946,7 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>12</v>
@@ -960,7 +960,7 @@
         <v>201</v>
       </c>
       <c r="C11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>11</v>
@@ -974,7 +974,7 @@
         <v>201</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>10</v>
@@ -988,10 +988,10 @@
         <v>201</v>
       </c>
       <c r="C13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -1002,10 +1002,10 @@
         <v>20101</v>
       </c>
       <c r="C14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F14" t="s">
         <v>21</v>
@@ -1019,7 +1019,7 @@
         <v>20101</v>
       </c>
       <c r="C15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>9</v>
@@ -1036,7 +1036,7 @@
         <v>2010101</v>
       </c>
       <c r="C16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>8</v>
@@ -1050,10 +1050,10 @@
         <v>20102</v>
       </c>
       <c r="C17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -1064,10 +1064,10 @@
         <v>2010201</v>
       </c>
       <c r="C18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -1078,10 +1078,10 @@
         <v>20103</v>
       </c>
       <c r="C19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F19" t="s">
         <v>35</v>
@@ -1095,10 +1095,10 @@
         <v>20103</v>
       </c>
       <c r="C20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F20" t="s">
         <v>4</v>
@@ -1112,10 +1112,10 @@
         <v>20104</v>
       </c>
       <c r="C21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F21" t="s">
         <v>3</v>
@@ -1129,10 +1129,10 @@
         <v>20104</v>
       </c>
       <c r="C22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F22" t="s">
         <v>2</v>
@@ -1146,10 +1146,10 @@
         <v>202</v>
       </c>
       <c r="C23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F23" t="s">
         <v>28</v>
@@ -1163,10 +1163,10 @@
         <v>202</v>
       </c>
       <c r="C24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F24" t="s">
         <v>27</v>
@@ -1180,10 +1180,10 @@
         <v>20201</v>
       </c>
       <c r="C25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F25" t="s">
         <v>25</v>
@@ -1197,10 +1197,10 @@
         <v>20201</v>
       </c>
       <c r="C26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F26" t="s">
         <v>6</v>
@@ -1214,10 +1214,10 @@
         <v>20203</v>
       </c>
       <c r="C27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -1242,10 +1242,10 @@
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F29" t="s">
         <v>7</v>
@@ -1259,10 +1259,10 @@
         <v>301</v>
       </c>
       <c r="C30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -1273,10 +1273,10 @@
         <v>302</v>
       </c>
       <c r="C31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -1287,10 +1287,10 @@
         <v>4</v>
       </c>
       <c r="C32" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F32" t="s">
         <v>36</v>
@@ -1304,10 +1304,10 @@
         <v>4</v>
       </c>
       <c r="C33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D33" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F33" t="s">
         <v>22</v>
@@ -1321,13 +1321,13 @@
         <v>5</v>
       </c>
       <c r="C34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D34" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -1338,10 +1338,10 @@
         <v>6</v>
       </c>
       <c r="C35" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D35" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F35" t="s">
         <v>26</v>
@@ -1355,10 +1355,10 @@
         <v>7</v>
       </c>
       <c r="C36" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -1369,10 +1369,10 @@
         <v>8</v>
       </c>
       <c r="C37" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D37" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F37" t="s">
         <v>23</v>
@@ -1386,10 +1386,10 @@
         <v>8</v>
       </c>
       <c r="C38" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F38" t="s">
         <v>4</v>
@@ -1403,10 +1403,10 @@
         <v>9</v>
       </c>
       <c r="C39" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D39" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F39" t="s">
         <v>34</v>
@@ -1420,10 +1420,10 @@
         <v>9</v>
       </c>
       <c r="C40" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D40" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F40" t="s">
         <v>32</v>
@@ -1437,10 +1437,10 @@
         <v>9</v>
       </c>
       <c r="C41" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F41" t="s">
         <v>33</v>
@@ -1454,10 +1454,10 @@
         <v>901</v>
       </c>
       <c r="C42" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D42" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F42" t="s">
         <v>30</v>
@@ -1471,10 +1471,10 @@
         <v>901</v>
       </c>
       <c r="C43" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D43" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F43" t="s">
         <v>31</v>
@@ -1488,10 +1488,10 @@
         <v>901</v>
       </c>
       <c r="C44" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D44" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F44" t="s">
         <v>29</v>
@@ -1505,10 +1505,10 @@
         <v>902</v>
       </c>
       <c r="C45" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D45" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F45" t="s">
         <v>37</v>
@@ -1522,10 +1522,10 @@
         <v>902</v>
       </c>
       <c r="C46" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D46" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F46" t="s">
         <v>26</v>
@@ -1539,10 +1539,10 @@
         <v>902</v>
       </c>
       <c r="C47" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D47" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F47" t="s">
         <v>24</v>
@@ -1556,10 +1556,10 @@
         <v>10</v>
       </c>
       <c r="C48" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D48" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F48" t="s">
         <v>22</v>
@@ -1573,10 +1573,10 @@
         <v>10</v>
       </c>
       <c r="C49" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D49" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F49" t="s">
         <v>39</v>
@@ -1590,10 +1590,10 @@
         <v>10</v>
       </c>
       <c r="C50" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D50" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F50" t="s">
         <v>38</v>
@@ -1607,10 +1607,10 @@
         <v>11</v>
       </c>
       <c r="C51" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F51" t="s">
         <v>0</v>
@@ -1624,10 +1624,10 @@
         <v>11</v>
       </c>
       <c r="C52" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F52" t="s">
         <v>1</v>
@@ -1641,10 +1641,10 @@
         <v>12</v>
       </c>
       <c r="C53" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F53" t="s">
         <v>21</v>
@@ -1658,10 +1658,10 @@
         <v>13</v>
       </c>
       <c r="C54" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
@@ -1672,10 +1672,10 @@
         <v>14</v>
       </c>
       <c r="C55" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D55" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
@@ -1686,10 +1686,10 @@
         <v>15</v>
       </c>
       <c r="C56" t="s">
+        <v>133</v>
+      </c>
+      <c r="D56" t="s">
         <v>134</v>
-      </c>
-      <c r="D56" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>